<commit_message>
20/02/2025: Added the select menu and the main menu
</commit_message>
<xml_diff>
--- a/localization/Localization.xlsx
+++ b/localization/Localization.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -27,6 +27,15 @@
     <t>es</t>
   </si>
   <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chain Reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reacción en cadena</t>
+  </si>
+  <si>
     <t>mm_play</t>
   </si>
   <si>
@@ -97,6 +106,33 @@
   </si>
   <si>
     <t xml:space="preserve">Menú principal</t>
+  </si>
+  <si>
+    <t>title_select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure the match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configura la partida</t>
+  </si>
+  <si>
+    <t>warn_select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The pieces have the same shape and color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las figuras tienen la misma forma y color</t>
+  </si>
+  <si>
+    <t>warn_ok</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Aceptar</t>
   </si>
 </sst>
 </file>
@@ -137,9 +173,10 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,8 +694,8 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="1" max="1" width="13.57421875"/>
-    <col customWidth="1" min="2" max="2" width="22.00390625"/>
-    <col bestFit="1" min="3" max="3" width="18.8515625"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" width="37.3828125"/>
+    <col bestFit="1" min="3" max="3" width="36.23046875"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -758,6 +795,50 @@
       </c>
       <c r="C9" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20/02/2025: Added an icon and refactored the code
</commit_message>
<xml_diff>
--- a/localization/Localization.xlsx
+++ b/localization/Localization.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -84,10 +84,10 @@
     <t>menu_win</t>
   </si>
   <si>
-    <t xml:space="preserve">Player {player} won!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¡Ha ganado el jugador {player}!</t>
+    <t xml:space="preserve">{player} won!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¡Ha ganado {player}!</t>
   </si>
   <si>
     <t>menu_revenge</t>
@@ -126,6 +126,15 @@
     <t xml:space="preserve">Las figuras tienen la misma forma y color</t>
   </si>
   <si>
+    <t>warn_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Both players must have a name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los dos jugadores deben tener nombre</t>
+  </si>
+  <si>
     <t>warn_ok</t>
   </si>
   <si>
@@ -133,6 +142,15 @@
   </si>
   <si>
     <t>Aceptar</t>
+  </si>
+  <si>
+    <t>name_enter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter name...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduce tu nombre...</t>
   </si>
 </sst>
 </file>
@@ -841,6 +859,28 @@
         <v>38</v>
       </c>
     </row>
+    <row r="14" ht="14.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>